<commit_message>
clean up project structure, added data for sync videos
</commit_message>
<xml_diff>
--- a/src/Auswertung.xlsx
+++ b/src/Auswertung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Desktop\GitHub\sa-objecttracking\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACED4FAF-3BB8-4A8A-9AA3-907D44E73C78}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB9768C-7137-42EC-880E-7BA9D26213FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12768" xr2:uid="{FF23FBBA-7FE2-413A-8DB7-381F64FAA2F6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>Perspektive</t>
   </si>
@@ -129,9 +129,6 @@
     <t>2_6</t>
   </si>
   <si>
-    <t>beide maxima summieren! Dann fast perfekt</t>
-  </si>
-  <si>
     <t>gut für Person vor Ball</t>
   </si>
   <si>
@@ -148,6 +145,24 @@
   </si>
   <si>
     <t>+++ = perfekt erkannt</t>
+  </si>
+  <si>
+    <t>csv done?</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>+ +</t>
+  </si>
+  <si>
+    <t>not neccessary</t>
+  </si>
+  <si>
+    <t>sehr einfaches Beispiel, gut für Bild von Trajectory</t>
+  </si>
+  <si>
+    <t>beide maxima summieren! Dann fast perfekt, Bild auch gutes Beispiel</t>
   </si>
 </sst>
 </file>
@@ -240,12 +255,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -259,34 +271,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -605,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB274E5-CBDC-4AC4-8072-DF364FB8AB0D}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,297 +635,345 @@
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="33.5546875" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" customWidth="1"/>
-    <col min="6" max="6" width="76.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
+    <col min="7" max="7" width="76.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="19.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:7" ht="19.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
-      <c r="B3" s="3" t="s">
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13"/>
+      <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="16"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13"/>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13"/>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="16"/>
+    </row>
+    <row r="8" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="1" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
+      <c r="B9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" t="s">
+      <c r="E9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="18"/>
+    </row>
+    <row r="10" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="16"/>
+    </row>
+    <row r="14" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="16"/>
+      <c r="B14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="16"/>
+    </row>
+    <row r="16" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
+      <c r="B17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
-      <c r="B7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16"/>
-      <c r="B8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="9" t="s">
+      <c r="D18" s="2"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="9" t="s">
+      <c r="D19" s="2"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="9" t="s">
+      <c r="D20" s="2"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="A10:A17"/>
-    <mergeCell ref="E2:E9"/>
-    <mergeCell ref="E10:E17"/>
+    <mergeCell ref="F2:F9"/>
+    <mergeCell ref="F10:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>